<commit_message>
Agregando botón de pedidos en tabla cotización
</commit_message>
<xml_diff>
--- a/assets/uploads/Formato_precios.xlsx
+++ b/assets/uploads/Formato_precios.xlsx
@@ -6138,7 +6138,10 @@
   <dimension ref="A1:D1704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>